<commit_message>
Display the spectrum title on the color info
</commit_message>
<xml_diff>
--- a/Extra/Tests/Window Layout.xlsx
+++ b/Extra/Tests/Window Layout.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9e8c9bfceb7de713/Documentos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9e8c9bfceb7de713/Documentos/Python/Projetos/CIE Chromaticity/Extra/Tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{0175EB05-10FA-4DEB-B00D-B593EB8D5B43}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{EAFB3CA0-3571-4049-BB89-B21D3AD28453}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{0175EB05-10FA-4DEB-B00D-B593EB8D5B43}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8B6DF54B-89B9-4BA3-A097-D7A944AA4948}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{172AA20B-51F1-427A-A2A8-55E096F8C03C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{172AA20B-51F1-427A-A2A8-55E096F8C03C}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Toolbar</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Spectral distribution</t>
+  </si>
+  <si>
+    <t>Spectrum name</t>
   </si>
 </sst>
 </file>
@@ -147,17 +150,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -166,7 +169,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -484,7 +490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6D068FC-8FA5-4579-BB87-DBCB1B539A3E}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -498,21 +504,21 @@
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="209.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -525,9 +531,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E97E141-C6F0-4BCA-AEB0-02F02CF8E838}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -536,55 +544,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="4" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="6" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:C5"/>
+  <mergeCells count="4">
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Spectral Distribution to the color info frame
</commit_message>
<xml_diff>
--- a/Extra/Tests/Window Layout.xlsx
+++ b/Extra/Tests/Window Layout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9e8c9bfceb7de713/Documentos/Python/Projetos/CIE Chromaticity/Extra/Tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{0175EB05-10FA-4DEB-B00D-B593EB8D5B43}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8B6DF54B-89B9-4BA3-A097-D7A944AA4948}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{0175EB05-10FA-4DEB-B00D-B593EB8D5B43}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D1F37FB1-18C5-42D4-BA35-F1A2148C9C76}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{172AA20B-51F1-427A-A2A8-55E096F8C03C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Toolbar</t>
   </si>
@@ -62,12 +62,6 @@
   </si>
   <si>
     <t>Color</t>
-  </si>
-  <si>
-    <t>R: nnn, G: nnn, B:nnn</t>
-  </si>
-  <si>
-    <t>#ffffff</t>
   </si>
   <si>
     <t xml:space="preserve"> Spectral distribution</t>
@@ -150,12 +144,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -167,9 +158,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -501,24 +489,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="5"/>
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="209.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -531,7 +519,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E97E141-C6F0-4BCA-AEB0-02F02CF8E838}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:C1"/>
@@ -544,11 +532,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="A1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -557,7 +545,7 @@
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -568,7 +556,7 @@
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -577,29 +565,19 @@
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="C2:C4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A5:C5"/>
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>